<commit_message>
💩 municipios en proceso
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/municipios_colombia.xlsx
+++ b/aplicaciones/procesador/datos/municipios_colombia.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$1:$J$683</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4768" uniqueCount="3414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4769" uniqueCount="3415">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -9094,9 +9095,6 @@
     <t xml:space="preserve">-1.0677332</t>
   </si>
   <si>
-    <t xml:space="preserve">-76.6138698</t>
-  </si>
-  <si>
     <t xml:space="preserve">Puerto Alegría</t>
   </si>
   <si>
@@ -10265,18 +10263,23 @@
   </si>
   <si>
     <t xml:space="preserve">-77.0293497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cucunubá</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -10320,12 +10323,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -10395,7 +10392,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10407,7 +10404,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10424,7 +10421,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
+          <fgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10432,7 +10429,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10444,126 +10441,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A842" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D871" activeCellId="0" sqref="D871"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A832" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E869" activeCellId="0" sqref="E869"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -35286,8 +35177,8 @@
       <c r="B728" s="0" t="s">
         <v>3022</v>
       </c>
-      <c r="C728" s="9" t="s">
-        <v>3023</v>
+      <c r="C728" s="9" t="n">
+        <v>-72.5156301</v>
       </c>
       <c r="D728" s="0" t="n">
         <v>91</v>
@@ -35297,13 +35188,13 @@
     </row>
     <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="0" t="s">
+        <v>3023</v>
+      </c>
+      <c r="B729" s="0" t="s">
         <v>3024</v>
       </c>
-      <c r="B729" s="0" t="s">
+      <c r="C729" s="9" t="s">
         <v>3025</v>
-      </c>
-      <c r="C729" s="9" t="s">
-        <v>3026</v>
       </c>
       <c r="D729" s="0" t="n">
         <v>91</v>
@@ -35313,13 +35204,13 @@
     </row>
     <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="0" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B730" s="0" t="s">
         <v>3027</v>
       </c>
-      <c r="B730" s="0" t="s">
+      <c r="C730" s="9" t="s">
         <v>3028</v>
-      </c>
-      <c r="C730" s="9" t="s">
-        <v>3029</v>
       </c>
       <c r="D730" s="0" t="n">
         <v>91</v>
@@ -35329,13 +35220,13 @@
     </row>
     <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="0" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B731" s="0" t="s">
         <v>3030</v>
       </c>
-      <c r="B731" s="0" t="s">
+      <c r="C731" s="9" t="s">
         <v>3031</v>
-      </c>
-      <c r="C731" s="9" t="s">
-        <v>3032</v>
       </c>
       <c r="D731" s="0" t="n">
         <v>88</v>
@@ -35345,13 +35236,13 @@
     </row>
     <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="0" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B732" s="0" t="s">
         <v>3033</v>
       </c>
-      <c r="B732" s="0" t="s">
+      <c r="C732" s="9" t="s">
         <v>3034</v>
-      </c>
-      <c r="C732" s="9" t="s">
-        <v>3035</v>
       </c>
       <c r="D732" s="0" t="n">
         <v>91</v>
@@ -35361,13 +35252,13 @@
     </row>
     <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="0" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B733" s="0" t="s">
         <v>3036</v>
       </c>
-      <c r="B733" s="0" t="s">
+      <c r="C733" s="9" t="s">
         <v>3037</v>
-      </c>
-      <c r="C733" s="9" t="s">
-        <v>3038</v>
       </c>
       <c r="D733" s="0" t="n">
         <v>52</v>
@@ -35377,13 +35268,13 @@
     </row>
     <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="0" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B734" s="0" t="s">
         <v>3039</v>
       </c>
-      <c r="B734" s="0" t="s">
+      <c r="C734" s="9" t="s">
         <v>3040</v>
-      </c>
-      <c r="C734" s="9" t="s">
-        <v>3041</v>
       </c>
       <c r="D734" s="0" t="n">
         <v>8</v>
@@ -35393,13 +35284,13 @@
     </row>
     <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="0" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B735" s="0" t="s">
         <v>3042</v>
       </c>
-      <c r="B735" s="0" t="s">
+      <c r="C735" s="9" t="s">
         <v>3043</v>
-      </c>
-      <c r="C735" s="9" t="s">
-        <v>3044</v>
       </c>
       <c r="D735" s="0" t="n">
         <v>54</v>
@@ -35409,13 +35300,13 @@
     </row>
     <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="0" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B736" s="0" t="s">
         <v>3045</v>
       </c>
-      <c r="B736" s="0" t="s">
+      <c r="C736" s="9" t="s">
         <v>3046</v>
-      </c>
-      <c r="C736" s="9" t="s">
-        <v>3047</v>
       </c>
       <c r="D736" s="0" t="n">
         <v>15</v>
@@ -35425,13 +35316,13 @@
     </row>
     <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="0" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B737" s="0" t="s">
         <v>3048</v>
       </c>
-      <c r="B737" s="0" t="s">
+      <c r="C737" s="9" t="s">
         <v>3049</v>
-      </c>
-      <c r="C737" s="9" t="s">
-        <v>3050</v>
       </c>
       <c r="D737" s="0" t="n">
         <v>15</v>
@@ -35441,13 +35332,13 @@
     </row>
     <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="0" t="s">
+        <v>3050</v>
+      </c>
+      <c r="B738" s="0" t="s">
         <v>3051</v>
       </c>
-      <c r="B738" s="0" t="s">
+      <c r="C738" s="9" t="s">
         <v>3052</v>
-      </c>
-      <c r="C738" s="9" t="s">
-        <v>3053</v>
       </c>
       <c r="D738" s="0" t="n">
         <v>15</v>
@@ -35457,13 +35348,13 @@
     </row>
     <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="0" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B739" s="0" t="s">
         <v>3054</v>
       </c>
-      <c r="B739" s="0" t="s">
+      <c r="C739" s="9" t="s">
         <v>3055</v>
-      </c>
-      <c r="C739" s="9" t="s">
-        <v>3056</v>
       </c>
       <c r="D739" s="0" t="n">
         <v>15</v>
@@ -35473,13 +35364,13 @@
     </row>
     <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="0" t="s">
+        <v>3056</v>
+      </c>
+      <c r="B740" s="0" t="s">
         <v>3057</v>
       </c>
-      <c r="B740" s="0" t="s">
+      <c r="C740" s="9" t="s">
         <v>3058</v>
-      </c>
-      <c r="C740" s="9" t="s">
-        <v>3059</v>
       </c>
       <c r="D740" s="0" t="n">
         <v>68</v>
@@ -35489,13 +35380,13 @@
     </row>
     <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="0" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B741" s="0" t="s">
         <v>3060</v>
       </c>
-      <c r="B741" s="0" t="s">
+      <c r="C741" s="9" t="s">
         <v>3061</v>
-      </c>
-      <c r="C741" s="9" t="s">
-        <v>3062</v>
       </c>
       <c r="D741" s="0" t="n">
         <v>91</v>
@@ -35508,10 +35399,10 @@
         <v>35</v>
       </c>
       <c r="B742" s="0" t="s">
+        <v>3062</v>
+      </c>
+      <c r="C742" s="9" t="s">
         <v>3063</v>
-      </c>
-      <c r="C742" s="9" t="s">
-        <v>3064</v>
       </c>
       <c r="D742" s="0" t="n">
         <v>25</v>
@@ -35521,13 +35412,13 @@
     </row>
     <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="0" t="s">
+        <v>3064</v>
+      </c>
+      <c r="B743" s="0" t="s">
         <v>3065</v>
       </c>
-      <c r="B743" s="0" t="s">
+      <c r="C743" s="9" t="s">
         <v>3066</v>
-      </c>
-      <c r="C743" s="9" t="s">
-        <v>3067</v>
       </c>
       <c r="D743" s="0" t="n">
         <v>68</v>
@@ -35537,13 +35428,13 @@
     </row>
     <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="0" t="s">
+        <v>3067</v>
+      </c>
+      <c r="B744" s="0" t="s">
         <v>3068</v>
       </c>
-      <c r="B744" s="0" t="s">
+      <c r="C744" s="9" t="s">
         <v>3069</v>
-      </c>
-      <c r="C744" s="9" t="s">
-        <v>3070</v>
       </c>
       <c r="D744" s="0" t="n">
         <v>52</v>
@@ -35556,10 +35447,10 @@
         <v>581</v>
       </c>
       <c r="B745" s="0" t="s">
+        <v>3070</v>
+      </c>
+      <c r="C745" s="9" t="s">
         <v>3071</v>
-      </c>
-      <c r="C745" s="9" t="s">
-        <v>3072</v>
       </c>
       <c r="D745" s="0" t="n">
         <v>5</v>
@@ -35569,13 +35460,13 @@
     </row>
     <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A746" s="0" t="s">
+        <v>3072</v>
+      </c>
+      <c r="B746" s="0" t="s">
         <v>3073</v>
       </c>
-      <c r="B746" s="0" t="s">
+      <c r="C746" s="9" t="s">
         <v>3074</v>
-      </c>
-      <c r="C746" s="9" t="s">
-        <v>3075</v>
       </c>
       <c r="D746" s="0" t="n">
         <v>52</v>
@@ -35585,13 +35476,13 @@
     </row>
     <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="0" t="s">
+        <v>3075</v>
+      </c>
+      <c r="B747" s="0" t="s">
         <v>3076</v>
       </c>
-      <c r="B747" s="0" t="s">
+      <c r="C747" s="9" t="s">
         <v>3077</v>
-      </c>
-      <c r="C747" s="9" t="s">
-        <v>3078</v>
       </c>
       <c r="D747" s="0" t="n">
         <v>94</v>
@@ -35601,13 +35492,13 @@
     </row>
     <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="0" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B748" s="0" t="s">
         <v>3079</v>
       </c>
-      <c r="B748" s="0" t="s">
+      <c r="C748" s="9" t="s">
         <v>3080</v>
-      </c>
-      <c r="C748" s="9" t="s">
-        <v>3081</v>
       </c>
       <c r="D748" s="0" t="n">
         <v>52</v>
@@ -35617,13 +35508,13 @@
     </row>
     <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="0" t="s">
+        <v>3081</v>
+      </c>
+      <c r="B749" s="0" t="s">
         <v>3082</v>
       </c>
-      <c r="B749" s="0" t="s">
+      <c r="C749" s="9" t="s">
         <v>3083</v>
-      </c>
-      <c r="C749" s="9" t="s">
-        <v>3084</v>
       </c>
       <c r="D749" s="0" t="n">
         <v>54</v>
@@ -35633,13 +35524,13 @@
     </row>
     <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="0" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B750" s="0" t="s">
         <v>3085</v>
       </c>
-      <c r="B750" s="0" t="s">
+      <c r="C750" s="9" t="s">
         <v>3086</v>
-      </c>
-      <c r="C750" s="9" t="s">
-        <v>3087</v>
       </c>
       <c r="D750" s="0" t="n">
         <v>54</v>
@@ -35649,13 +35540,13 @@
     </row>
     <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="0" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B751" s="0" t="s">
         <v>3088</v>
       </c>
-      <c r="B751" s="0" t="s">
+      <c r="C751" s="9" t="s">
         <v>3089</v>
-      </c>
-      <c r="C751" s="9" t="s">
-        <v>3090</v>
       </c>
       <c r="D751" s="0" t="n">
         <v>68</v>
@@ -35665,13 +35556,13 @@
     </row>
     <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A752" s="0" t="s">
+        <v>3090</v>
+      </c>
+      <c r="B752" s="0" t="s">
         <v>3091</v>
       </c>
-      <c r="B752" s="0" t="s">
+      <c r="C752" s="9" t="s">
         <v>3092</v>
-      </c>
-      <c r="C752" s="9" t="s">
-        <v>3093</v>
       </c>
       <c r="D752" s="0" t="n">
         <v>54</v>
@@ -35681,13 +35572,13 @@
     </row>
     <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A753" s="0" t="s">
+        <v>3093</v>
+      </c>
+      <c r="B753" s="0" t="s">
         <v>3094</v>
       </c>
-      <c r="B753" s="0" t="s">
+      <c r="C753" s="9" t="s">
         <v>3095</v>
-      </c>
-      <c r="C753" s="9" t="s">
-        <v>3096</v>
       </c>
       <c r="D753" s="0" t="n">
         <v>25</v>
@@ -35697,13 +35588,13 @@
     </row>
     <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A754" s="0" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B754" s="0" t="s">
         <v>3097</v>
       </c>
-      <c r="B754" s="0" t="s">
+      <c r="C754" s="9" t="s">
         <v>3098</v>
-      </c>
-      <c r="C754" s="9" t="s">
-        <v>3099</v>
       </c>
       <c r="D754" s="0" t="n">
         <v>5</v>
@@ -35713,13 +35604,13 @@
     </row>
     <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A755" s="0" t="s">
+        <v>3099</v>
+      </c>
+      <c r="B755" s="0" t="s">
         <v>3100</v>
       </c>
-      <c r="B755" s="0" t="s">
+      <c r="C755" s="9" t="s">
         <v>3101</v>
-      </c>
-      <c r="C755" s="9" t="s">
-        <v>3102</v>
       </c>
       <c r="D755" s="0" t="n">
         <v>52</v>
@@ -35729,13 +35620,13 @@
     </row>
     <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="0" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B756" s="0" t="s">
         <v>3103</v>
       </c>
-      <c r="B756" s="0" t="s">
+      <c r="C756" s="9" t="s">
         <v>3104</v>
-      </c>
-      <c r="C756" s="9" t="s">
-        <v>3105</v>
       </c>
       <c r="D756" s="0" t="n">
         <v>73</v>
@@ -35748,10 +35639,10 @@
         <v>35</v>
       </c>
       <c r="B757" s="0" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C757" s="9" t="s">
         <v>3106</v>
-      </c>
-      <c r="C757" s="9" t="s">
-        <v>3107</v>
       </c>
       <c r="D757" s="0" t="n">
         <v>52</v>
@@ -35761,13 +35652,13 @@
     </row>
     <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A758" s="0" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B758" s="0" t="s">
         <v>3108</v>
       </c>
-      <c r="B758" s="0" t="s">
+      <c r="C758" s="9" t="s">
         <v>3109</v>
-      </c>
-      <c r="C758" s="9" t="s">
-        <v>3110</v>
       </c>
       <c r="D758" s="0" t="n">
         <v>52</v>
@@ -35777,13 +35668,13 @@
     </row>
     <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A759" s="0" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B759" s="0" t="s">
         <v>3111</v>
       </c>
-      <c r="B759" s="0" t="s">
+      <c r="C759" s="9" t="s">
         <v>3112</v>
-      </c>
-      <c r="C759" s="9" t="s">
-        <v>3113</v>
       </c>
       <c r="D759" s="0" t="n">
         <v>52</v>
@@ -35793,13 +35684,13 @@
     </row>
     <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A760" s="0" t="s">
+        <v>3113</v>
+      </c>
+      <c r="B760" s="0" t="s">
         <v>3114</v>
       </c>
-      <c r="B760" s="0" t="s">
+      <c r="C760" s="9" t="s">
         <v>3115</v>
-      </c>
-      <c r="C760" s="9" t="s">
-        <v>3116</v>
       </c>
       <c r="D760" s="0" t="n">
         <v>19</v>
@@ -35812,10 +35703,10 @@
         <v>1105</v>
       </c>
       <c r="B761" s="0" t="s">
+        <v>3116</v>
+      </c>
+      <c r="C761" s="9" t="s">
         <v>3117</v>
-      </c>
-      <c r="C761" s="9" t="s">
-        <v>3118</v>
       </c>
       <c r="D761" s="0" t="n">
         <v>5</v>
@@ -35825,13 +35716,13 @@
     </row>
     <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A762" s="0" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B762" s="0" t="s">
         <v>3119</v>
       </c>
-      <c r="B762" s="0" t="s">
+      <c r="C762" s="9" t="s">
         <v>3120</v>
-      </c>
-      <c r="C762" s="9" t="s">
-        <v>3121</v>
       </c>
       <c r="D762" s="2" t="n">
         <v>54</v>
@@ -35841,13 +35732,13 @@
     </row>
     <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A763" s="0" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B763" s="0" t="s">
         <v>3122</v>
       </c>
-      <c r="B763" s="0" t="s">
+      <c r="C763" s="9" t="s">
         <v>3123</v>
-      </c>
-      <c r="C763" s="9" t="s">
-        <v>3124</v>
       </c>
       <c r="D763" s="0" t="n">
         <v>54</v>
@@ -35857,13 +35748,13 @@
     </row>
     <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A764" s="0" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B764" s="0" t="s">
         <v>3125</v>
       </c>
-      <c r="B764" s="0" t="s">
+      <c r="C764" s="9" t="s">
         <v>3126</v>
-      </c>
-      <c r="C764" s="9" t="s">
-        <v>3127</v>
       </c>
       <c r="D764" s="0" t="n">
         <v>52</v>
@@ -35873,13 +35764,13 @@
     </row>
     <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A765" s="0" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B765" s="0" t="s">
         <v>3128</v>
       </c>
-      <c r="B765" s="0" t="s">
+      <c r="C765" s="9" t="s">
         <v>3129</v>
-      </c>
-      <c r="C765" s="9" t="s">
-        <v>3130</v>
       </c>
       <c r="D765" s="0" t="n">
         <v>54</v>
@@ -35889,13 +35780,13 @@
     </row>
     <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A766" s="0" t="s">
+        <v>3130</v>
+      </c>
+      <c r="B766" s="0" t="s">
         <v>3131</v>
       </c>
-      <c r="B766" s="0" t="s">
+      <c r="C766" s="9" t="s">
         <v>3132</v>
-      </c>
-      <c r="C766" s="9" t="s">
-        <v>3133</v>
       </c>
       <c r="D766" s="0" t="n">
         <v>54</v>
@@ -35905,13 +35796,13 @@
     </row>
     <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A767" s="0" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B767" s="0" t="s">
         <v>3134</v>
       </c>
-      <c r="B767" s="0" t="s">
+      <c r="C767" s="9" t="s">
         <v>3135</v>
-      </c>
-      <c r="C767" s="9" t="s">
-        <v>3136</v>
       </c>
       <c r="D767" s="0" t="n">
         <v>54</v>
@@ -35921,13 +35812,13 @@
     </row>
     <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A768" s="0" t="s">
+        <v>3136</v>
+      </c>
+      <c r="B768" s="0" t="s">
         <v>3137</v>
       </c>
-      <c r="B768" s="0" t="s">
+      <c r="C768" s="9" t="s">
         <v>3138</v>
-      </c>
-      <c r="C768" s="9" t="s">
-        <v>3139</v>
       </c>
       <c r="D768" s="0" t="n">
         <v>5</v>
@@ -35937,13 +35828,13 @@
     </row>
     <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A769" s="0" t="s">
+        <v>3139</v>
+      </c>
+      <c r="B769" s="0" t="s">
         <v>3140</v>
       </c>
-      <c r="B769" s="0" t="s">
+      <c r="C769" s="9" t="s">
         <v>3141</v>
-      </c>
-      <c r="C769" s="9" t="s">
-        <v>3142</v>
       </c>
       <c r="D769" s="0" t="n">
         <v>25</v>
@@ -35953,13 +35844,13 @@
     </row>
     <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A770" s="0" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B770" s="0" t="s">
         <v>3143</v>
       </c>
-      <c r="B770" s="0" t="s">
+      <c r="C770" s="9" t="s">
         <v>3144</v>
-      </c>
-      <c r="C770" s="9" t="s">
-        <v>3145</v>
       </c>
       <c r="D770" s="0" t="n">
         <v>5</v>
@@ -35969,13 +35860,13 @@
     </row>
     <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A771" s="0" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B771" s="0" t="s">
         <v>3146</v>
       </c>
-      <c r="B771" s="0" t="s">
+      <c r="C771" s="9" t="s">
         <v>3147</v>
-      </c>
-      <c r="C771" s="9" t="s">
-        <v>3148</v>
       </c>
       <c r="D771" s="0" t="n">
         <v>52</v>
@@ -35985,13 +35876,13 @@
     </row>
     <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A772" s="0" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B772" s="0" t="s">
         <v>3149</v>
       </c>
-      <c r="B772" s="0" t="s">
+      <c r="C772" s="9" t="s">
         <v>3150</v>
-      </c>
-      <c r="C772" s="9" t="s">
-        <v>3151</v>
       </c>
       <c r="D772" s="0" t="n">
         <v>50</v>
@@ -36001,13 +35892,13 @@
     </row>
     <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A773" s="0" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B773" s="0" t="s">
         <v>3152</v>
       </c>
-      <c r="B773" s="0" t="s">
+      <c r="C773" s="9" t="s">
         <v>3153</v>
-      </c>
-      <c r="C773" s="9" t="s">
-        <v>3154</v>
       </c>
       <c r="D773" s="0" t="n">
         <v>94</v>
@@ -36017,13 +35908,13 @@
     </row>
     <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A774" s="0" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B774" s="0" t="s">
         <v>3155</v>
       </c>
-      <c r="B774" s="0" t="s">
+      <c r="C774" s="9" t="s">
         <v>3156</v>
-      </c>
-      <c r="C774" s="9" t="s">
-        <v>3157</v>
       </c>
       <c r="D774" s="0" t="n">
         <v>27</v>
@@ -36033,13 +35924,13 @@
     </row>
     <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A775" s="0" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B775" s="0" t="s">
         <v>3158</v>
       </c>
-      <c r="B775" s="0" t="s">
+      <c r="C775" s="9" t="s">
         <v>3159</v>
-      </c>
-      <c r="C775" s="9" t="s">
-        <v>3160</v>
       </c>
       <c r="D775" s="0" t="n">
         <v>68</v>
@@ -36052,10 +35943,10 @@
         <v>227</v>
       </c>
       <c r="B776" s="0" t="s">
+        <v>3160</v>
+      </c>
+      <c r="C776" s="9" t="s">
         <v>3161</v>
-      </c>
-      <c r="C776" s="9" t="s">
-        <v>3162</v>
       </c>
       <c r="D776" s="0" t="n">
         <v>19</v>
@@ -36065,13 +35956,13 @@
     </row>
     <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A777" s="0" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B777" s="0" t="s">
         <v>3163</v>
       </c>
-      <c r="B777" s="0" t="s">
+      <c r="C777" s="9" t="s">
         <v>3164</v>
-      </c>
-      <c r="C777" s="9" t="s">
-        <v>3165</v>
       </c>
       <c r="D777" s="0" t="n">
         <v>25</v>
@@ -36081,13 +35972,13 @@
     </row>
     <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A778" s="0" t="s">
+        <v>3165</v>
+      </c>
+      <c r="B778" s="0" t="s">
         <v>3166</v>
       </c>
-      <c r="B778" s="0" t="s">
+      <c r="C778" s="9" t="s">
         <v>3167</v>
-      </c>
-      <c r="C778" s="9" t="s">
-        <v>3168</v>
       </c>
       <c r="D778" s="0" t="n">
         <v>25</v>
@@ -36097,13 +35988,13 @@
     </row>
     <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A779" s="0" t="s">
+        <v>3168</v>
+      </c>
+      <c r="B779" s="0" t="s">
         <v>3169</v>
       </c>
-      <c r="B779" s="0" t="s">
+      <c r="C779" s="9" t="s">
         <v>3170</v>
-      </c>
-      <c r="C779" s="9" t="s">
-        <v>3171</v>
       </c>
       <c r="D779" s="0" t="n">
         <v>94</v>
@@ -36113,13 +36004,13 @@
     </row>
     <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A780" s="0" t="s">
+        <v>3171</v>
+      </c>
+      <c r="B780" s="0" t="s">
         <v>3172</v>
       </c>
-      <c r="B780" s="0" t="s">
+      <c r="C780" s="9" t="s">
         <v>3173</v>
-      </c>
-      <c r="C780" s="9" t="s">
-        <v>3174</v>
       </c>
       <c r="D780" s="0" t="n">
         <v>15</v>
@@ -36129,13 +36020,13 @@
     </row>
     <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A781" s="0" t="s">
+        <v>3174</v>
+      </c>
+      <c r="B781" s="0" t="s">
         <v>3175</v>
       </c>
-      <c r="B781" s="0" t="s">
+      <c r="C781" s="9" t="s">
         <v>3176</v>
-      </c>
-      <c r="C781" s="9" t="s">
-        <v>3177</v>
       </c>
       <c r="D781" s="0" t="n">
         <v>27</v>
@@ -36145,13 +36036,13 @@
     </row>
     <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A782" s="0" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B782" s="0" t="s">
         <v>3178</v>
       </c>
-      <c r="B782" s="0" t="s">
+      <c r="C782" s="9" t="s">
         <v>3179</v>
-      </c>
-      <c r="C782" s="9" t="s">
-        <v>3180</v>
       </c>
       <c r="D782" s="0" t="n">
         <v>5</v>
@@ -36161,13 +36052,13 @@
     </row>
     <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A783" s="0" t="s">
+        <v>3180</v>
+      </c>
+      <c r="B783" s="0" t="s">
         <v>3181</v>
       </c>
-      <c r="B783" s="0" t="s">
+      <c r="C783" s="9" t="s">
         <v>3182</v>
-      </c>
-      <c r="C783" s="9" t="s">
-        <v>3183</v>
       </c>
       <c r="D783" s="0" t="n">
         <v>68</v>
@@ -36180,10 +36071,10 @@
         <v>2730</v>
       </c>
       <c r="B784" s="0" t="s">
+        <v>3183</v>
+      </c>
+      <c r="C784" s="9" t="s">
         <v>3184</v>
-      </c>
-      <c r="C784" s="9" t="s">
-        <v>3185</v>
       </c>
       <c r="D784" s="0" t="n">
         <v>15</v>
@@ -36196,10 +36087,10 @@
         <v>357</v>
       </c>
       <c r="B785" s="0" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C785" s="9" t="s">
         <v>3186</v>
-      </c>
-      <c r="C785" s="9" t="s">
-        <v>3187</v>
       </c>
       <c r="D785" s="0" t="n">
         <v>68</v>
@@ -36209,13 +36100,13 @@
     </row>
     <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A786" s="0" t="s">
+        <v>3187</v>
+      </c>
+      <c r="B786" s="0" t="s">
         <v>3188</v>
       </c>
-      <c r="B786" s="0" t="s">
+      <c r="C786" s="9" t="s">
         <v>3189</v>
-      </c>
-      <c r="C786" s="9" t="s">
-        <v>3190</v>
       </c>
       <c r="D786" s="0" t="n">
         <v>54</v>
@@ -36225,13 +36116,13 @@
     </row>
     <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A787" s="0" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B787" s="0" t="s">
         <v>3191</v>
       </c>
-      <c r="B787" s="0" t="s">
+      <c r="C787" s="9" t="s">
         <v>3192</v>
-      </c>
-      <c r="C787" s="9" t="s">
-        <v>3193</v>
       </c>
       <c r="D787" s="0" t="n">
         <v>25</v>
@@ -36241,13 +36132,13 @@
     </row>
     <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A788" s="0" t="s">
+        <v>3193</v>
+      </c>
+      <c r="B788" s="0" t="s">
         <v>3194</v>
       </c>
-      <c r="B788" s="0" t="s">
+      <c r="C788" s="9" t="s">
         <v>3195</v>
-      </c>
-      <c r="C788" s="9" t="s">
-        <v>3196</v>
       </c>
       <c r="D788" s="0" t="n">
         <v>15</v>
@@ -36257,13 +36148,13 @@
     </row>
     <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A789" s="0" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B789" s="0" t="s">
         <v>3197</v>
       </c>
-      <c r="B789" s="0" t="s">
+      <c r="C789" s="9" t="s">
         <v>3198</v>
-      </c>
-      <c r="C789" s="9" t="s">
-        <v>3199</v>
       </c>
       <c r="D789" s="0" t="n">
         <v>15</v>
@@ -36273,13 +36164,13 @@
     </row>
     <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A790" s="0" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B790" s="0" t="s">
         <v>3200</v>
       </c>
-      <c r="B790" s="0" t="s">
+      <c r="C790" s="9" t="s">
         <v>3201</v>
-      </c>
-      <c r="C790" s="9" t="s">
-        <v>3202</v>
       </c>
       <c r="D790" s="0" t="n">
         <v>52</v>
@@ -36289,13 +36180,13 @@
     </row>
     <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A791" s="0" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B791" s="0" t="s">
         <v>3203</v>
       </c>
-      <c r="B791" s="0" t="s">
+      <c r="C791" s="9" t="s">
         <v>3204</v>
-      </c>
-      <c r="C791" s="9" t="s">
-        <v>3205</v>
       </c>
       <c r="D791" s="0" t="n">
         <v>25</v>
@@ -36305,13 +36196,13 @@
     </row>
     <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A792" s="0" t="s">
+        <v>3205</v>
+      </c>
+      <c r="B792" s="0" t="s">
         <v>3206</v>
       </c>
-      <c r="B792" s="0" t="s">
+      <c r="C792" s="9" t="s">
         <v>3207</v>
-      </c>
-      <c r="C792" s="9" t="s">
-        <v>3208</v>
       </c>
       <c r="D792" s="0" t="n">
         <v>54</v>
@@ -36321,13 +36212,13 @@
     </row>
     <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A793" s="0" t="s">
+        <v>3208</v>
+      </c>
+      <c r="B793" s="0" t="s">
         <v>3209</v>
       </c>
-      <c r="B793" s="0" t="s">
+      <c r="C793" s="9" t="s">
         <v>3210</v>
-      </c>
-      <c r="C793" s="9" t="s">
-        <v>3211</v>
       </c>
       <c r="D793" s="0" t="n">
         <v>52</v>
@@ -36337,13 +36228,13 @@
     </row>
     <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A794" s="0" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B794" s="0" t="s">
         <v>3212</v>
       </c>
-      <c r="B794" s="0" t="s">
+      <c r="C794" s="9" t="s">
         <v>3213</v>
-      </c>
-      <c r="C794" s="9" t="s">
-        <v>3214</v>
       </c>
       <c r="D794" s="0" t="n">
         <v>52</v>
@@ -36353,13 +36244,13 @@
     </row>
     <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A795" s="0" t="s">
+        <v>3214</v>
+      </c>
+      <c r="B795" s="0" t="s">
         <v>3215</v>
       </c>
-      <c r="B795" s="0" t="s">
+      <c r="C795" s="9" t="s">
         <v>3216</v>
-      </c>
-      <c r="C795" s="9" t="s">
-        <v>3217</v>
       </c>
       <c r="D795" s="0" t="n">
         <v>52</v>
@@ -36369,13 +36260,13 @@
     </row>
     <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A796" s="0" t="s">
+        <v>3217</v>
+      </c>
+      <c r="B796" s="0" t="s">
         <v>3218</v>
       </c>
-      <c r="B796" s="0" t="s">
+      <c r="C796" s="9" t="s">
         <v>3219</v>
-      </c>
-      <c r="C796" s="9" t="s">
-        <v>3220</v>
       </c>
       <c r="D796" s="0" t="n">
         <v>54</v>
@@ -36385,13 +36276,13 @@
     </row>
     <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A797" s="0" t="s">
+        <v>3220</v>
+      </c>
+      <c r="B797" s="0" t="s">
         <v>3221</v>
       </c>
-      <c r="B797" s="0" t="s">
+      <c r="C797" s="9" t="s">
         <v>3222</v>
-      </c>
-      <c r="C797" s="9" t="s">
-        <v>3223</v>
       </c>
       <c r="D797" s="0" t="n">
         <v>25</v>
@@ -36401,13 +36292,13 @@
     </row>
     <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A798" s="0" t="s">
+        <v>3223</v>
+      </c>
+      <c r="B798" s="0" t="s">
         <v>3224</v>
       </c>
-      <c r="B798" s="0" t="s">
+      <c r="C798" s="9" t="s">
         <v>3225</v>
-      </c>
-      <c r="C798" s="9" t="s">
-        <v>3226</v>
       </c>
       <c r="D798" s="0" t="n">
         <v>5</v>
@@ -36417,13 +36308,13 @@
     </row>
     <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A799" s="0" t="s">
+        <v>3226</v>
+      </c>
+      <c r="B799" s="0" t="s">
         <v>3227</v>
       </c>
-      <c r="B799" s="0" t="s">
+      <c r="C799" s="9" t="s">
         <v>3228</v>
-      </c>
-      <c r="C799" s="9" t="s">
-        <v>3229</v>
       </c>
       <c r="D799" s="0" t="n">
         <v>15</v>
@@ -36433,13 +36324,13 @@
     </row>
     <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A800" s="0" t="s">
+        <v>3229</v>
+      </c>
+      <c r="B800" s="0" t="s">
         <v>3230</v>
       </c>
-      <c r="B800" s="0" t="s">
+      <c r="C800" s="9" t="s">
         <v>3231</v>
-      </c>
-      <c r="C800" s="9" t="s">
-        <v>3232</v>
       </c>
       <c r="D800" s="0" t="n">
         <v>15</v>
@@ -36449,13 +36340,13 @@
     </row>
     <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A801" s="0" t="s">
+        <v>3232</v>
+      </c>
+      <c r="B801" s="0" t="s">
         <v>3233</v>
       </c>
-      <c r="B801" s="0" t="s">
+      <c r="C801" s="9" t="s">
         <v>3234</v>
-      </c>
-      <c r="C801" s="9" t="s">
-        <v>3235</v>
       </c>
       <c r="D801" s="0" t="n">
         <v>15</v>
@@ -36465,13 +36356,13 @@
     </row>
     <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A802" s="0" t="s">
+        <v>3235</v>
+      </c>
+      <c r="B802" s="0" t="s">
         <v>3236</v>
       </c>
-      <c r="B802" s="0" t="s">
+      <c r="C802" s="9" t="s">
         <v>3237</v>
-      </c>
-      <c r="C802" s="9" t="s">
-        <v>3238</v>
       </c>
       <c r="D802" s="0" t="n">
         <v>25</v>
@@ -36481,13 +36372,13 @@
     </row>
     <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A803" s="0" t="s">
+        <v>3238</v>
+      </c>
+      <c r="B803" s="0" t="s">
         <v>3239</v>
       </c>
-      <c r="B803" s="0" t="s">
+      <c r="C803" s="0" t="s">
         <v>3240</v>
-      </c>
-      <c r="C803" s="0" t="s">
-        <v>3241</v>
       </c>
       <c r="D803" s="0" t="n">
         <v>54</v>
@@ -36500,10 +36391,10 @@
         <v>1711</v>
       </c>
       <c r="B804" s="0" t="s">
+        <v>3241</v>
+      </c>
+      <c r="C804" s="0" t="s">
         <v>3242</v>
-      </c>
-      <c r="C804" s="0" t="s">
-        <v>3243</v>
       </c>
       <c r="D804" s="0" t="n">
         <v>27</v>
@@ -36513,13 +36404,13 @@
     </row>
     <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A805" s="0" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B805" s="0" t="s">
         <v>3244</v>
       </c>
-      <c r="B805" s="0" t="s">
+      <c r="C805" s="0" t="s">
         <v>3245</v>
-      </c>
-      <c r="C805" s="0" t="s">
-        <v>3246</v>
       </c>
       <c r="D805" s="0" t="n">
         <v>25</v>
@@ -36529,13 +36420,13 @@
     </row>
     <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A806" s="0" t="s">
-        <v>3036</v>
+        <v>3035</v>
       </c>
       <c r="B806" s="0" t="s">
+        <v>3246</v>
+      </c>
+      <c r="C806" s="0" t="s">
         <v>3247</v>
-      </c>
-      <c r="C806" s="0" t="s">
-        <v>3248</v>
       </c>
       <c r="D806" s="0" t="n">
         <v>25</v>
@@ -36545,13 +36436,13 @@
     </row>
     <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A807" s="0" t="s">
+        <v>3248</v>
+      </c>
+      <c r="B807" s="0" t="s">
         <v>3249</v>
       </c>
-      <c r="B807" s="0" t="s">
+      <c r="C807" s="0" t="s">
         <v>3250</v>
-      </c>
-      <c r="C807" s="0" t="s">
-        <v>3251</v>
       </c>
       <c r="D807" s="0" t="n">
         <v>68</v>
@@ -36561,13 +36452,13 @@
     </row>
     <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A808" s="0" t="s">
+        <v>3251</v>
+      </c>
+      <c r="B808" s="0" t="s">
         <v>3252</v>
       </c>
-      <c r="B808" s="0" t="s">
+      <c r="C808" s="0" t="s">
         <v>3253</v>
-      </c>
-      <c r="C808" s="0" t="s">
-        <v>3254</v>
       </c>
       <c r="D808" s="0" t="n">
         <v>81</v>
@@ -36577,13 +36468,13 @@
     </row>
     <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A809" s="0" t="s">
+        <v>3254</v>
+      </c>
+      <c r="B809" s="0" t="s">
         <v>3255</v>
       </c>
-      <c r="B809" s="0" t="s">
+      <c r="C809" s="0" t="s">
         <v>3256</v>
-      </c>
-      <c r="C809" s="0" t="s">
-        <v>3257</v>
       </c>
       <c r="D809" s="0" t="n">
         <v>15</v>
@@ -36593,13 +36484,13 @@
     </row>
     <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A810" s="0" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B810" s="0" t="s">
         <v>3258</v>
       </c>
-      <c r="B810" s="0" t="s">
+      <c r="C810" s="0" t="s">
         <v>3259</v>
-      </c>
-      <c r="C810" s="0" t="s">
-        <v>3260</v>
       </c>
       <c r="D810" s="0" t="n">
         <v>52</v>
@@ -36609,13 +36500,13 @@
     </row>
     <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A811" s="0" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B811" s="0" t="s">
         <v>3261</v>
       </c>
-      <c r="B811" s="0" t="s">
+      <c r="C811" s="0" t="s">
         <v>3262</v>
-      </c>
-      <c r="C811" s="0" t="s">
-        <v>3263</v>
       </c>
       <c r="D811" s="0" t="n">
         <v>54</v>
@@ -36625,13 +36516,13 @@
     </row>
     <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A812" s="0" t="s">
+        <v>3263</v>
+      </c>
+      <c r="B812" s="0" t="s">
         <v>3264</v>
       </c>
-      <c r="B812" s="0" t="s">
+      <c r="C812" s="0" t="s">
         <v>3265</v>
-      </c>
-      <c r="C812" s="0" t="s">
-        <v>3266</v>
       </c>
       <c r="D812" s="0" t="n">
         <v>68</v>
@@ -36641,13 +36532,13 @@
     </row>
     <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A813" s="0" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B813" s="0" t="s">
         <v>3267</v>
       </c>
-      <c r="B813" s="0" t="s">
+      <c r="C813" s="0" t="s">
         <v>3268</v>
-      </c>
-      <c r="C813" s="0" t="s">
-        <v>3269</v>
       </c>
       <c r="D813" s="0" t="n">
         <v>68</v>
@@ -36657,13 +36548,13 @@
     </row>
     <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A814" s="0" t="s">
+        <v>3269</v>
+      </c>
+      <c r="B814" s="0" t="s">
         <v>3270</v>
       </c>
-      <c r="B814" s="0" t="s">
+      <c r="C814" s="0" t="s">
         <v>3271</v>
-      </c>
-      <c r="C814" s="0" t="s">
-        <v>3272</v>
       </c>
       <c r="D814" s="0" t="n">
         <v>15</v>
@@ -36673,13 +36564,13 @@
     </row>
     <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A815" s="0" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B815" s="0" t="s">
         <v>3273</v>
       </c>
-      <c r="B815" s="0" t="s">
+      <c r="C815" s="0" t="s">
         <v>3274</v>
-      </c>
-      <c r="C815" s="0" t="s">
-        <v>3275</v>
       </c>
       <c r="D815" s="0" t="n">
         <v>27</v>
@@ -36689,13 +36580,13 @@
     </row>
     <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="0" t="s">
+        <v>3275</v>
+      </c>
+      <c r="B816" s="0" t="s">
         <v>3276</v>
       </c>
-      <c r="B816" s="0" t="s">
+      <c r="C816" s="0" t="s">
         <v>3277</v>
-      </c>
-      <c r="C816" s="0" t="s">
-        <v>3278</v>
       </c>
       <c r="D816" s="0" t="n">
         <v>68</v>
@@ -36705,13 +36596,13 @@
     </row>
     <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A817" s="0" t="s">
+        <v>3278</v>
+      </c>
+      <c r="B817" s="0" t="s">
         <v>3279</v>
       </c>
-      <c r="B817" s="0" t="s">
+      <c r="C817" s="0" t="s">
         <v>3280</v>
-      </c>
-      <c r="C817" s="0" t="s">
-        <v>3281</v>
       </c>
       <c r="D817" s="0" t="n">
         <v>25</v>
@@ -36721,13 +36612,13 @@
     </row>
     <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A818" s="0" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B818" s="0" t="s">
         <v>3282</v>
       </c>
-      <c r="B818" s="0" t="s">
+      <c r="C818" s="0" t="s">
         <v>3283</v>
-      </c>
-      <c r="C818" s="0" t="s">
-        <v>3284</v>
       </c>
       <c r="D818" s="0" t="n">
         <v>68</v>
@@ -36737,13 +36628,13 @@
     </row>
     <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A819" s="0" t="s">
+        <v>3284</v>
+      </c>
+      <c r="B819" s="0" t="s">
         <v>3285</v>
       </c>
-      <c r="B819" s="0" t="s">
+      <c r="C819" s="0" t="s">
         <v>3286</v>
-      </c>
-      <c r="C819" s="0" t="s">
-        <v>3287</v>
       </c>
       <c r="D819" s="0" t="n">
         <v>15</v>
@@ -36753,13 +36644,13 @@
     </row>
     <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="0" t="s">
+        <v>3287</v>
+      </c>
+      <c r="B820" s="0" t="s">
         <v>3288</v>
       </c>
-      <c r="B820" s="0" t="s">
+      <c r="C820" s="0" t="s">
         <v>3289</v>
-      </c>
-      <c r="C820" s="0" t="s">
-        <v>3290</v>
       </c>
       <c r="D820" s="0" t="n">
         <v>25</v>
@@ -36769,13 +36660,13 @@
     </row>
     <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A821" s="0" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B821" s="0" t="s">
         <v>3291</v>
       </c>
-      <c r="B821" s="0" t="s">
+      <c r="C821" s="0" t="s">
         <v>3292</v>
-      </c>
-      <c r="C821" s="0" t="s">
-        <v>3293</v>
       </c>
       <c r="D821" s="0" t="n">
         <v>54</v>
@@ -36785,13 +36676,13 @@
     </row>
     <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A822" s="0" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B822" s="0" t="s">
         <v>3294</v>
       </c>
-      <c r="B822" s="0" t="s">
+      <c r="C822" s="0" t="s">
         <v>3295</v>
-      </c>
-      <c r="C822" s="0" t="s">
-        <v>3296</v>
       </c>
       <c r="D822" s="0" t="n">
         <v>27</v>
@@ -36804,10 +36695,10 @@
         <v>2425</v>
       </c>
       <c r="B823" s="0" t="s">
+        <v>3296</v>
+      </c>
+      <c r="C823" s="0" t="s">
         <v>3297</v>
-      </c>
-      <c r="C823" s="0" t="s">
-        <v>3298</v>
       </c>
       <c r="D823" s="0" t="n">
         <v>5</v>
@@ -36817,13 +36708,13 @@
     </row>
     <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A824" s="0" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B824" s="0" t="s">
         <v>3299</v>
       </c>
-      <c r="B824" s="0" t="s">
+      <c r="C824" s="0" t="s">
         <v>3300</v>
-      </c>
-      <c r="C824" s="0" t="s">
-        <v>3301</v>
       </c>
       <c r="D824" s="0" t="n">
         <v>44</v>
@@ -36833,13 +36724,13 @@
     </row>
     <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A825" s="0" t="s">
+        <v>3301</v>
+      </c>
+      <c r="B825" s="0" t="s">
         <v>3302</v>
       </c>
-      <c r="B825" s="0" t="s">
+      <c r="C825" s="0" t="s">
         <v>3303</v>
-      </c>
-      <c r="C825" s="0" t="s">
-        <v>3304</v>
       </c>
       <c r="D825" s="0" t="n">
         <v>25</v>
@@ -36849,13 +36740,13 @@
     </row>
     <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A826" s="0" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B826" s="0" t="s">
         <v>3305</v>
       </c>
-      <c r="B826" s="0" t="s">
+      <c r="C826" s="0" t="s">
         <v>3306</v>
-      </c>
-      <c r="C826" s="0" t="s">
-        <v>3307</v>
       </c>
       <c r="D826" s="0" t="n">
         <v>47</v>
@@ -36865,13 +36756,13 @@
     </row>
     <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A827" s="0" t="s">
+        <v>3307</v>
+      </c>
+      <c r="B827" s="0" t="s">
         <v>3308</v>
       </c>
-      <c r="B827" s="0" t="s">
+      <c r="C827" s="0" t="s">
         <v>3309</v>
-      </c>
-      <c r="C827" s="0" t="s">
-        <v>3310</v>
       </c>
       <c r="D827" s="0" t="n">
         <v>52</v>
@@ -36881,13 +36772,13 @@
     </row>
     <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A828" s="0" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B828" s="0" t="s">
         <v>3311</v>
       </c>
-      <c r="B828" s="0" t="s">
+      <c r="C828" s="0" t="s">
         <v>3312</v>
-      </c>
-      <c r="C828" s="0" t="s">
-        <v>3313</v>
       </c>
       <c r="D828" s="0" t="n">
         <v>52</v>
@@ -36897,13 +36788,13 @@
     </row>
     <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A829" s="0" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B829" s="0" t="s">
         <v>3314</v>
       </c>
-      <c r="B829" s="0" t="s">
+      <c r="C829" s="0" t="s">
         <v>3315</v>
-      </c>
-      <c r="C829" s="0" t="s">
-        <v>3316</v>
       </c>
       <c r="D829" s="0" t="n">
         <v>85</v>
@@ -36913,13 +36804,13 @@
     </row>
     <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A830" s="0" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B830" s="0" t="s">
         <v>3317</v>
       </c>
-      <c r="B830" s="0" t="s">
+      <c r="C830" s="0" t="s">
         <v>3318</v>
-      </c>
-      <c r="C830" s="0" t="s">
-        <v>3319</v>
       </c>
       <c r="D830" s="0" t="n">
         <v>27</v>
@@ -36929,13 +36820,13 @@
     </row>
     <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A831" s="0" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B831" s="0" t="s">
         <v>3320</v>
       </c>
-      <c r="B831" s="0" t="s">
+      <c r="C831" s="0" t="s">
         <v>3321</v>
-      </c>
-      <c r="C831" s="0" t="s">
-        <v>3322</v>
       </c>
       <c r="D831" s="0" t="n">
         <v>15</v>
@@ -36945,13 +36836,13 @@
     </row>
     <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A832" s="0" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B832" s="0" t="s">
         <v>3323</v>
       </c>
-      <c r="B832" s="0" t="s">
+      <c r="C832" s="0" t="s">
         <v>3324</v>
-      </c>
-      <c r="C832" s="0" t="s">
-        <v>3325</v>
       </c>
       <c r="D832" s="0" t="n">
         <v>68</v>
@@ -36961,13 +36852,13 @@
     </row>
     <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A833" s="0" t="s">
+        <v>3325</v>
+      </c>
+      <c r="B833" s="0" t="s">
         <v>3326</v>
       </c>
-      <c r="B833" s="0" t="s">
+      <c r="C833" s="0" t="s">
         <v>3327</v>
-      </c>
-      <c r="C833" s="0" t="s">
-        <v>3328</v>
       </c>
       <c r="D833" s="0" t="n">
         <v>52</v>
@@ -36977,13 +36868,13 @@
     </row>
     <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A834" s="0" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B834" s="0" t="s">
         <v>3329</v>
       </c>
-      <c r="B834" s="0" t="s">
+      <c r="C834" s="0" t="s">
         <v>3330</v>
-      </c>
-      <c r="C834" s="0" t="s">
-        <v>3331</v>
       </c>
       <c r="D834" s="0" t="n">
         <v>23</v>
@@ -36996,10 +36887,10 @@
         <v>344</v>
       </c>
       <c r="B835" s="0" t="s">
+        <v>3331</v>
+      </c>
+      <c r="C835" s="0" t="s">
         <v>3332</v>
-      </c>
-      <c r="C835" s="0" t="s">
-        <v>3333</v>
       </c>
       <c r="D835" s="0" t="n">
         <v>15</v>
@@ -37012,10 +36903,10 @@
         <v>2396</v>
       </c>
       <c r="B836" s="0" t="s">
+        <v>3333</v>
+      </c>
+      <c r="C836" s="0" t="s">
         <v>3334</v>
-      </c>
-      <c r="C836" s="0" t="s">
-        <v>3335</v>
       </c>
       <c r="D836" s="0" t="n">
         <v>15</v>
@@ -37025,13 +36916,13 @@
     </row>
     <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A837" s="0" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B837" s="0" t="s">
         <v>3336</v>
       </c>
-      <c r="B837" s="0" t="s">
+      <c r="C837" s="0" t="s">
         <v>3337</v>
-      </c>
-      <c r="C837" s="0" t="s">
-        <v>3338</v>
       </c>
       <c r="D837" s="0" t="n">
         <v>54</v>
@@ -37041,13 +36932,13 @@
     </row>
     <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A838" s="0" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B838" s="0" t="s">
         <v>3339</v>
       </c>
-      <c r="B838" s="0" t="s">
+      <c r="C838" s="0" t="s">
         <v>3340</v>
-      </c>
-      <c r="C838" s="0" t="s">
-        <v>3341</v>
       </c>
       <c r="D838" s="0" t="n">
         <v>68</v>
@@ -37057,13 +36948,13 @@
     </row>
     <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A839" s="0" t="s">
+        <v>3341</v>
+      </c>
+      <c r="B839" s="0" t="s">
         <v>3342</v>
       </c>
-      <c r="B839" s="0" t="s">
+      <c r="C839" s="0" t="s">
         <v>3343</v>
-      </c>
-      <c r="C839" s="0" t="s">
-        <v>3344</v>
       </c>
       <c r="D839" s="0" t="n">
         <v>54</v>
@@ -37073,13 +36964,13 @@
     </row>
     <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A840" s="0" t="s">
+        <v>3344</v>
+      </c>
+      <c r="B840" s="0" t="s">
         <v>3345</v>
       </c>
-      <c r="B840" s="0" t="s">
+      <c r="C840" s="0" t="s">
         <v>3346</v>
-      </c>
-      <c r="C840" s="0" t="s">
-        <v>3347</v>
       </c>
       <c r="D840" s="0" t="n">
         <v>50</v>
@@ -37089,13 +36980,13 @@
     </row>
     <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A841" s="0" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B841" s="0" t="s">
         <v>3348</v>
       </c>
-      <c r="B841" s="0" t="s">
+      <c r="C841" s="0" t="s">
         <v>3349</v>
-      </c>
-      <c r="C841" s="0" t="s">
-        <v>3350</v>
       </c>
       <c r="D841" s="0" t="n">
         <v>25</v>
@@ -37105,13 +36996,13 @@
     </row>
     <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A842" s="0" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="B842" s="0" t="s">
+        <v>3350</v>
+      </c>
+      <c r="C842" s="0" t="s">
         <v>3351</v>
-      </c>
-      <c r="C842" s="0" t="s">
-        <v>3352</v>
       </c>
       <c r="D842" s="0" t="n">
         <v>25</v>
@@ -37121,13 +37012,13 @@
     </row>
     <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A843" s="0" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B843" s="0" t="s">
         <v>3353</v>
       </c>
-      <c r="B843" s="0" t="s">
+      <c r="C843" s="0" t="s">
         <v>3354</v>
-      </c>
-      <c r="C843" s="0" t="s">
-        <v>3355</v>
       </c>
       <c r="D843" s="0" t="n">
         <v>25</v>
@@ -37137,13 +37028,13 @@
     </row>
     <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A844" s="0" t="s">
-        <v>3342</v>
+        <v>3341</v>
       </c>
       <c r="B844" s="0" t="s">
+        <v>3355</v>
+      </c>
+      <c r="C844" s="0" t="s">
         <v>3356</v>
-      </c>
-      <c r="C844" s="0" t="s">
-        <v>3357</v>
       </c>
       <c r="D844" s="0" t="n">
         <v>25</v>
@@ -37153,13 +37044,13 @@
     </row>
     <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A845" s="0" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B845" s="0" t="s">
         <v>3358</v>
       </c>
-      <c r="B845" s="0" t="s">
+      <c r="C845" s="0" t="s">
         <v>3359</v>
-      </c>
-      <c r="C845" s="0" t="s">
-        <v>3360</v>
       </c>
       <c r="D845" s="0" t="n">
         <v>5</v>
@@ -37169,13 +37060,13 @@
     </row>
     <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A846" s="0" t="s">
+        <v>3360</v>
+      </c>
+      <c r="B846" s="0" t="s">
         <v>3361</v>
       </c>
-      <c r="B846" s="0" t="s">
+      <c r="C846" s="0" t="s">
         <v>3362</v>
-      </c>
-      <c r="C846" s="0" t="s">
-        <v>3363</v>
       </c>
       <c r="D846" s="0" t="n">
         <v>68</v>
@@ -37188,10 +37079,10 @@
         <v>500</v>
       </c>
       <c r="B847" s="0" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C847" s="0" t="s">
         <v>3364</v>
-      </c>
-      <c r="C847" s="0" t="s">
-        <v>3365</v>
       </c>
       <c r="D847" s="0" t="n">
         <v>19</v>
@@ -37201,13 +37092,13 @@
     </row>
     <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A848" s="0" t="s">
+        <v>3365</v>
+      </c>
+      <c r="B848" s="0" t="s">
         <v>3366</v>
       </c>
-      <c r="B848" s="0" t="s">
+      <c r="C848" s="0" t="s">
         <v>3367</v>
-      </c>
-      <c r="C848" s="0" t="s">
-        <v>3368</v>
       </c>
       <c r="D848" s="0" t="n">
         <v>15</v>
@@ -37217,13 +37108,13 @@
     </row>
     <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A849" s="0" t="s">
-        <v>3137</v>
+        <v>3136</v>
       </c>
       <c r="B849" s="0" t="s">
+        <v>3368</v>
+      </c>
+      <c r="C849" s="0" t="s">
         <v>3369</v>
-      </c>
-      <c r="C849" s="0" t="s">
-        <v>3370</v>
       </c>
       <c r="D849" s="0" t="n">
         <v>86</v>
@@ -37233,13 +37124,13 @@
     </row>
     <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A850" s="0" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B850" s="0" t="s">
         <v>3371</v>
       </c>
-      <c r="B850" s="0" t="s">
+      <c r="C850" s="0" t="s">
         <v>3372</v>
-      </c>
-      <c r="C850" s="0" t="s">
-        <v>3373</v>
       </c>
       <c r="D850" s="0" t="n">
         <v>27</v>
@@ -37249,13 +37140,13 @@
     </row>
     <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A851" s="0" t="s">
+        <v>3373</v>
+      </c>
+      <c r="B851" s="0" t="s">
         <v>3374</v>
       </c>
-      <c r="B851" s="0" t="s">
+      <c r="C851" s="0" t="s">
         <v>3375</v>
-      </c>
-      <c r="C851" s="0" t="s">
-        <v>3376</v>
       </c>
       <c r="D851" s="0" t="n">
         <v>25</v>
@@ -37265,13 +37156,13 @@
     </row>
     <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A852" s="0" t="s">
+        <v>3376</v>
+      </c>
+      <c r="B852" s="0" t="s">
         <v>3377</v>
       </c>
-      <c r="B852" s="0" t="s">
+      <c r="C852" s="0" t="s">
         <v>3378</v>
-      </c>
-      <c r="C852" s="0" t="s">
-        <v>3379</v>
       </c>
       <c r="D852" s="0" t="n">
         <v>68</v>
@@ -37284,10 +37175,10 @@
         <v>625</v>
       </c>
       <c r="B853" s="0" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C853" s="0" t="s">
         <v>3380</v>
-      </c>
-      <c r="C853" s="0" t="s">
-        <v>3381</v>
       </c>
       <c r="D853" s="0" t="n">
         <v>15</v>
@@ -37297,13 +37188,13 @@
     </row>
     <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A854" s="0" t="s">
+        <v>3381</v>
+      </c>
+      <c r="B854" s="0" t="s">
         <v>3382</v>
       </c>
-      <c r="B854" s="0" t="s">
+      <c r="C854" s="0" t="s">
         <v>3383</v>
-      </c>
-      <c r="C854" s="0" t="s">
-        <v>3384</v>
       </c>
       <c r="D854" s="0" t="n">
         <v>15</v>
@@ -37313,13 +37204,13 @@
     </row>
     <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A855" s="0" t="s">
+        <v>3384</v>
+      </c>
+      <c r="B855" s="0" t="s">
         <v>3385</v>
       </c>
-      <c r="B855" s="0" t="s">
+      <c r="C855" s="0" t="s">
         <v>3386</v>
-      </c>
-      <c r="C855" s="0" t="s">
-        <v>3387</v>
       </c>
       <c r="D855" s="0" t="n">
         <v>52</v>
@@ -37329,13 +37220,13 @@
     </row>
     <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A856" s="0" t="s">
+        <v>3387</v>
+      </c>
+      <c r="B856" s="0" t="s">
         <v>3388</v>
       </c>
-      <c r="B856" s="0" t="s">
+      <c r="C856" s="0" t="s">
         <v>3389</v>
-      </c>
-      <c r="C856" s="0" t="s">
-        <v>3390</v>
       </c>
       <c r="D856" s="0" t="n">
         <v>52</v>
@@ -37345,13 +37236,13 @@
     </row>
     <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="0" t="s">
+        <v>3390</v>
+      </c>
+      <c r="B857" s="0" t="s">
         <v>3391</v>
       </c>
-      <c r="B857" s="0" t="s">
+      <c r="C857" s="0" t="s">
         <v>3392</v>
-      </c>
-      <c r="C857" s="0" t="s">
-        <v>3393</v>
       </c>
       <c r="D857" s="0" t="n">
         <v>52</v>
@@ -37361,13 +37252,13 @@
     </row>
     <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A858" s="0" t="s">
+        <v>3393</v>
+      </c>
+      <c r="B858" s="0" t="s">
         <v>3394</v>
       </c>
-      <c r="B858" s="0" t="s">
+      <c r="C858" s="0" t="s">
         <v>3395</v>
-      </c>
-      <c r="C858" s="0" t="s">
-        <v>3396</v>
       </c>
       <c r="D858" s="0" t="n">
         <v>52</v>
@@ -37377,13 +37268,13 @@
     </row>
     <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A859" s="0" t="s">
+        <v>3396</v>
+      </c>
+      <c r="B859" s="0" t="s">
         <v>3397</v>
       </c>
-      <c r="B859" s="0" t="s">
+      <c r="C859" s="0" t="s">
         <v>3398</v>
-      </c>
-      <c r="C859" s="0" t="s">
-        <v>3399</v>
       </c>
       <c r="D859" s="0" t="n">
         <v>52</v>
@@ -37396,10 +37287,10 @@
         <v>1961</v>
       </c>
       <c r="B860" s="0" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C860" s="0" t="s">
         <v>3400</v>
-      </c>
-      <c r="C860" s="0" t="s">
-        <v>3401</v>
       </c>
       <c r="D860" s="0" t="n">
         <v>52</v>
@@ -37409,13 +37300,13 @@
     </row>
     <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A861" s="0" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B861" s="0" t="s">
         <v>3402</v>
       </c>
-      <c r="B861" s="0" t="s">
+      <c r="C861" s="0" t="s">
         <v>3403</v>
-      </c>
-      <c r="C861" s="0" t="s">
-        <v>3404</v>
       </c>
       <c r="D861" s="0" t="n">
         <v>52</v>
@@ -37425,13 +37316,13 @@
     </row>
     <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A862" s="0" t="s">
+        <v>3404</v>
+      </c>
+      <c r="B862" s="0" t="s">
         <v>3405</v>
       </c>
-      <c r="B862" s="0" t="s">
+      <c r="C862" s="0" t="s">
         <v>3406</v>
-      </c>
-      <c r="C862" s="0" t="s">
-        <v>3407</v>
       </c>
       <c r="D862" s="0" t="n">
         <v>52</v>
@@ -37441,13 +37332,13 @@
     </row>
     <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A863" s="0" t="s">
+        <v>3407</v>
+      </c>
+      <c r="B863" s="0" t="s">
         <v>3408</v>
       </c>
-      <c r="B863" s="0" t="s">
+      <c r="C863" s="0" t="s">
         <v>3409</v>
-      </c>
-      <c r="C863" s="0" t="s">
-        <v>3410</v>
       </c>
       <c r="D863" s="0" t="n">
         <v>52</v>
@@ -37457,13 +37348,13 @@
     </row>
     <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A864" s="0" t="s">
+        <v>3410</v>
+      </c>
+      <c r="B864" s="0" t="s">
         <v>3411</v>
       </c>
-      <c r="B864" s="0" t="s">
+      <c r="C864" s="0" t="s">
         <v>3412</v>
-      </c>
-      <c r="C864" s="0" t="s">
-        <v>3413</v>
       </c>
       <c r="D864" s="0" t="n">
         <v>52</v>
@@ -37472,10 +37363,34 @@
       <c r="F864" s="7"/>
     </row>
     <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A865" s="0" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B865" s="0" t="n">
+        <v>0.2000471</v>
+      </c>
+      <c r="C865" s="0" t="n">
+        <v>-71.7014844</v>
+      </c>
+      <c r="D865" s="0" t="n">
+        <v>97</v>
+      </c>
       <c r="E865" s="7"/>
       <c r="F865" s="7"/>
     </row>
     <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A866" s="0" t="s">
+        <v>3414</v>
+      </c>
+      <c r="B866" s="0" t="n">
+        <v>5.2505183</v>
+      </c>
+      <c r="C866" s="0" t="n">
+        <v>-73.7694433</v>
+      </c>
+      <c r="D866" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="E866" s="7"/>
       <c r="F866" s="7"/>
     </row>
@@ -38022,4 +37937,27 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>